<commit_message>
spanish/hungarian templates added - inited - tbc
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_tob_en.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_tob_en.xlsx
@@ -160,13 +160,13 @@
     <t>For questions please contact the FoodRisk-Labs team, +49 (30) 18412-4444, foodrisklabs@bfr.bund.de</t>
   </si>
   <si>
-    <t>In Column A starting with Line Number x please enter the line number of the outgoing good being the product of this ingredient. Afterwards, enter ingredient information in columns B to M.</t>
-  </si>
-  <si>
     <t>Then, please assess the data for the next outgoing good(s) accordingly.</t>
   </si>
   <si>
     <t>Digital extracts (e.g. Excel or XML files) of the company database could also be suitable. In this case you do not need to fill this template - please call us to find a solution (BfR FoodRiskLabs-Team, +49 (30) 18412-4444)</t>
+  </si>
+  <si>
+    <t>In Column A starting with Line Number x please enter the line number of the outgoing good being the product of this ingredient. Afterwards, enter the requested information into columns B onwards.</t>
   </si>
 </sst>
 </file>
@@ -1549,6 +1549,40 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="38" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1557,6 +1591,117 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="30" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="30" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="30" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1578,162 +1723,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="30" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="30" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="30" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="38" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="114">
@@ -2178,137 +2178,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="38" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="83"/>
       <c r="K1" s="39"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="70"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
       <c r="O1" s="37"/>
       <c r="P1" s="37"/>
       <c r="Q1" s="37"/>
       <c r="R1" s="37"/>
     </row>
     <row r="2" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="59"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="75"/>
     </row>
     <row r="3" spans="1:18" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="87"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="47"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
     <row r="4" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="51" t="s">
+      <c r="E4" s="61"/>
+      <c r="F4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="53" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="91" t="s">
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="56" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="93"/>
-      <c r="B5" s="73" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="73" t="s">
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="K5" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="91"/>
+      <c r="N5" s="56"/>
     </row>
     <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="95"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2318,12 +2318,12 @@
       <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="56"/>
     </row>
     <row r="7" spans="1:18" s="7" customFormat="1" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
@@ -2348,202 +2348,202 @@
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="90"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="52"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
     </row>
     <row r="9" spans="1:18" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="52"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="55"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
     </row>
     <row r="10" spans="1:18" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="52"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="55"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
     </row>
     <row r="11" spans="1:18" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="52"/>
+      <c r="A11" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
     </row>
     <row r="12" spans="1:18" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="52"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
     </row>
     <row r="13" spans="1:18" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
+      <c r="A13" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="87"/>
       <c r="O13" s="40"/>
       <c r="P13" s="40"/>
       <c r="Q13" s="40"/>
       <c r="R13" s="41"/>
     </row>
     <row r="14" spans="1:18" s="42" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="48"/>
+      <c r="A14" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="90"/>
       <c r="O14" s="40"/>
       <c r="P14" s="40"/>
       <c r="Q14" s="40"/>
       <c r="R14" s="41"/>
     </row>
     <row r="15" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="80"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:18" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="76" t="s">
+      <c r="E16" s="48"/>
+      <c r="F16" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="81" t="s">
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="91" t="s">
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="56" t="s">
         <v>13</v>
       </c>
       <c r="O16" s="16"/>
@@ -2552,51 +2552,51 @@
       <c r="R16" s="16"/>
     </row>
     <row r="17" spans="1:18" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="93"/>
-      <c r="B17" s="74" t="s">
+      <c r="A17" s="58"/>
+      <c r="B17" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="76" t="s">
+      <c r="F17" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="74" t="s">
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="71" t="s">
+      <c r="K17" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="71" t="s">
+      <c r="L17" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="83" t="s">
+      <c r="M17" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="N17" s="91"/>
+      <c r="N17" s="56"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
     <row r="18" spans="1:18" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="94"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2606,12 +2606,12 @@
       <c r="H18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="75"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="84"/>
-      <c r="N18" s="92"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="57"/>
       <c r="O18" s="16"/>
       <c r="P18" s="16"/>
       <c r="Q18" s="16"/>
@@ -3003,6 +3003,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A13:N13"/>
+    <mergeCell ref="A14:N14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A12:N12"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="J16:M16"/>
     <mergeCell ref="M17:M18"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="C17:C18"/>
@@ -3019,36 +3049,6 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="A15:N15"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A13:N13"/>
-    <mergeCell ref="A14:N14"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A12:N12"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7 F15 F3 F19:F1048576">

</xml_diff>